<commit_message>
Implementing Select Date feature
</commit_message>
<xml_diff>
--- a/Data/ConfigData/SalarySlipConfig.xlsx
+++ b/Data/ConfigData/SalarySlipConfig.xlsx
@@ -91,10 +91,10 @@
     <t>NewSalary</t>
   </si>
   <si>
+    <t>ResSalarySlip</t>
+  </si>
+  <si>
     <t>DepSalarySlip</t>
-  </si>
-  <si>
-    <t>ResSalarySlip</t>
   </si>
 </sst>
 </file>
@@ -102,10 +102,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -239,30 +239,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,6 +380,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -399,60 +453,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,12 +581,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -608,7 +608,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -638,22 +638,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -665,25 +665,25 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -692,13 +692,13 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -719,7 +719,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1048,8 +1048,8 @@
   <sheetPr/>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
@@ -1155,23 +1155,8 @@
       <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="2">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>3</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>24</v>
@@ -1186,7 +1171,7 @@
         <v>3</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>24</v>
@@ -1235,11 +1220,21 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>

</xml_diff>